<commit_message>
Updated effort (Worked on state diagram, reasoned on requirements)
</commit_message>
<xml_diff>
--- a/Effort/EffortGiulioAbbo.xlsx
+++ b/Effort/EffortGiulioAbbo.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/IS2proj/AbboAccordiBonetti/Effort/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giulio Antonio Abbo\Google Drive\Poli\SE project\Effort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FAC0E1-E657-AD48-A286-E25AD56F8C02}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E649A0-36D3-4E67-A500-69C5119EEAB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0B28E5B0-B43E-E940-AC9B-200C96DB78B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Giulio Abbo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Purpose, scope, definitions</t>
   </si>
@@ -64,6 +61,15 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>(+1)</t>
+  </si>
+  <si>
+    <t>Giulio A. Abbo</t>
   </si>
 </sst>
 </file>
@@ -107,16 +113,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -132,7 +141,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -428,89 +437,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2283A0BD-A3F0-6040-B65F-FBDAEAD5CFA1}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B3:B11)</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -518,5 +551,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>